<commit_message>
Sync from private branch main
</commit_message>
<xml_diff>
--- a/data-exploration-demo/weather_data.xlsx
+++ b/data-exploration-demo/weather_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,14 +466,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-06-26T23:00:00+00:00/PT1H</t>
+          <t>2025-06-27T11:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>23.88888888888889</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D2" t="n">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3">
@@ -482,14 +482,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-27T00:00:00+00:00/PT2H</t>
+          <t>2025-06-27T12:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>23.33333333333333</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D3" t="n">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
@@ -498,14 +498,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-06-27T02:00:00+00:00/PT1H</t>
+          <t>2025-06-27T14:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>22.22222222222222</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D4" t="n">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
@@ -514,14 +514,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-06-27T03:00:00+00:00/PT1H</t>
+          <t>2025-06-27T15:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>20.55555555555556</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D5" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6">
@@ -530,14 +530,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-06-27T04:00:00+00:00/PT2H</t>
+          <t>2025-06-27T16:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>20.55555555555556</v>
       </c>
       <c r="D6" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
@@ -546,14 +546,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2025-06-27T06:00:00+00:00/PT4H</t>
+          <t>2025-06-27T17:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>19.44444444444444</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="D7" t="n">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8">
@@ -562,14 +562,14 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2025-06-27T10:00:00+00:00/PT2H</t>
+          <t>2025-06-27T18:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18.33333333333333</v>
+        <v>23.88888888888889</v>
       </c>
       <c r="D8" t="n">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -578,14 +578,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2025-06-27T12:00:00+00:00/PT2H</t>
+          <t>2025-06-27T19:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17.77777777777778</v>
+        <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10">
@@ -594,14 +594,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-06-27T14:00:00+00:00/PT1H</t>
+          <t>2025-06-27T20:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18.33333333333333</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D10" t="n">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
@@ -610,14 +610,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-06-27T15:00:00+00:00/PT1H</t>
+          <t>2025-06-27T21:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>18.88888888888889</v>
+        <v>26.66666666666667</v>
       </c>
       <c r="D11" t="n">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12">
@@ -626,14 +626,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-06-27T16:00:00+00:00/PT1H</t>
+          <t>2025-06-27T22:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D12" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
@@ -642,14 +642,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-06-27T17:00:00+00:00/PT1H</t>
+          <t>2025-06-27T23:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>21.66666666666667</v>
+        <v>25</v>
       </c>
       <c r="D13" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
@@ -658,14 +658,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-06-27T18:00:00+00:00/PT1H</t>
+          <t>2025-06-28T00:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>22.22222222222222</v>
+        <v>23.88888888888889</v>
       </c>
       <c r="D14" t="n">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -674,7 +674,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-06-27T19:00:00+00:00/PT1H</t>
+          <t>2025-06-28T01:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -690,14 +690,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-06-27T20:00:00+00:00/PT1H</t>
+          <t>2025-06-28T02:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>24.44444444444444</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="D16" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -706,14 +706,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2025-06-27T21:00:00+00:00/PT1H</t>
+          <t>2025-06-28T03:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>25</v>
+        <v>20.55555555555556</v>
       </c>
       <c r="D17" t="n">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
@@ -722,14 +722,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2025-06-27T22:00:00+00:00/PT1H</t>
+          <t>2025-06-28T04:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>24.44444444444444</v>
+        <v>20</v>
       </c>
       <c r="D18" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19">
@@ -738,14 +738,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2025-06-27T23:00:00+00:00/PT2H</t>
+          <t>2025-06-28T05:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>23.33333333333333</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D19" t="n">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20">
@@ -754,14 +754,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2025-06-28T01:00:00+00:00/PT1H</t>
+          <t>2025-06-28T07:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>22.22222222222222</v>
+        <v>18.88888888888889</v>
       </c>
       <c r="D20" t="n">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
@@ -770,14 +770,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-06-28T02:00:00+00:00/PT1H</t>
+          <t>2025-06-28T08:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20.55555555555556</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D21" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22">
@@ -786,14 +786,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-06-28T03:00:00+00:00/PT1H</t>
+          <t>2025-06-28T10:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D22" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23">
@@ -802,14 +802,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2025-06-28T04:00:00+00:00/PT3H</t>
+          <t>2025-06-28T12:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>19.44444444444444</v>
+        <v>17.22222222222222</v>
       </c>
       <c r="D23" t="n">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24">
@@ -818,14 +818,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2025-06-28T07:00:00+00:00/PT1H</t>
+          <t>2025-06-28T14:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>18.88888888888889</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D24" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
@@ -834,14 +834,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2025-06-28T08:00:00+00:00/PT2H</t>
+          <t>2025-06-28T15:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>18.33333333333333</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D25" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26">
@@ -850,14 +850,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2025-06-28T10:00:00+00:00/PT1H</t>
+          <t>2025-06-28T16:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>17.77777777777778</v>
+        <v>20.55555555555556</v>
       </c>
       <c r="D26" t="n">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27">
@@ -866,14 +866,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2025-06-28T11:00:00+00:00/PT3H</t>
+          <t>2025-06-28T17:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17.22222222222222</v>
+        <v>22.77777777777778</v>
       </c>
       <c r="D27" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
@@ -882,14 +882,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2025-06-28T14:00:00+00:00/PT1H</t>
+          <t>2025-06-28T18:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>17.77777777777778</v>
+        <v>25</v>
       </c>
       <c r="D28" t="n">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29">
@@ -898,14 +898,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2025-06-28T15:00:00+00:00/PT1H</t>
+          <t>2025-06-28T19:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>19.44444444444444</v>
+        <v>27.22222222222222</v>
       </c>
       <c r="D29" t="n">
-        <v>67</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30">
@@ -914,14 +914,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2025-06-28T16:00:00+00:00/PT1H</t>
+          <t>2025-06-28T20:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>21.11111111111111</v>
+        <v>27.77777777777778</v>
       </c>
       <c r="D30" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31">
@@ -930,14 +930,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2025-06-28T17:00:00+00:00/PT1H</t>
+          <t>2025-06-28T21:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>24.44444444444444</v>
+        <v>27.22222222222222</v>
       </c>
       <c r="D31" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32">
@@ -946,7 +946,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2025-06-28T18:00:00+00:00/PT1H</t>
+          <t>2025-06-28T22:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -962,14 +962,14 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2025-06-28T19:00:00+00:00/PT3H</t>
+          <t>2025-06-28T23:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>28.88888888888889</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D33" t="n">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34">
@@ -978,14 +978,14 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2025-06-28T22:00:00+00:00/PT1H</t>
+          <t>2025-06-29T00:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>28.33333333333333</v>
+        <v>24.44444444444444</v>
       </c>
       <c r="D34" t="n">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35">
@@ -994,14 +994,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2025-06-28T23:00:00+00:00/PT1H</t>
+          <t>2025-06-29T01:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27.77777777777778</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="D35" t="n">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36">
@@ -1010,14 +1010,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2025-06-29T00:00:00+00:00/PT1H</t>
+          <t>2025-06-29T02:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>26.66666666666667</v>
+        <v>21.11111111111111</v>
       </c>
       <c r="D36" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37">
@@ -1026,14 +1026,14 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2025-06-29T01:00:00+00:00/PT1H</t>
+          <t>2025-06-29T03:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>24.44444444444444</v>
+        <v>20</v>
       </c>
       <c r="D37" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38">
@@ -1042,14 +1042,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2025-06-29T02:00:00+00:00/PT1H</t>
+          <t>2025-06-29T04:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>22.22222222222222</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D38" t="n">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39">
@@ -1058,14 +1058,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2025-06-29T03:00:00+00:00/PT1H</t>
+          <t>2025-06-29T05:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>20.55555555555556</v>
+        <v>18.88888888888889</v>
       </c>
       <c r="D39" t="n">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40">
@@ -1074,14 +1074,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2025-06-29T04:00:00+00:00/PT1H</t>
+          <t>2025-06-29T07:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>19.44444444444444</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D40" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41">
@@ -1090,14 +1090,14 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2025-06-29T05:00:00+00:00/PT1H</t>
+          <t>2025-06-29T09:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>18.88888888888889</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D41" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42">
@@ -1106,14 +1106,14 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2025-06-29T06:00:00+00:00/PT3H</t>
+          <t>2025-06-29T11:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>18.33333333333333</v>
+        <v>17.22222222222222</v>
       </c>
       <c r="D42" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43">
@@ -1122,14 +1122,14 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2025-06-29T09:00:00+00:00/PT2H</t>
+          <t>2025-06-29T13:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>17.77777777777778</v>
+        <v>16.66666666666667</v>
       </c>
       <c r="D43" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2025-06-29T11:00:00+00:00/PT3H</t>
+          <t>2025-06-29T15:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1154,14 +1154,14 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2025-06-29T14:00:00+00:00/PT1H</t>
+          <t>2025-06-29T16:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>17.77777777777778</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D45" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46">
@@ -1170,14 +1170,14 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2025-06-29T15:00:00+00:00/PT1H</t>
+          <t>2025-06-29T17:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>18.33333333333333</v>
+        <v>20.55555555555556</v>
       </c>
       <c r="D46" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47">
@@ -1186,14 +1186,14 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2025-06-29T16:00:00+00:00/PT1H</t>
+          <t>2025-06-29T18:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>20</v>
+        <v>23.33333333333333</v>
       </c>
       <c r="D47" t="n">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48">
@@ -1202,14 +1202,14 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2025-06-29T17:00:00+00:00/PT1H</t>
+          <t>2025-06-29T19:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>21.66666666666667</v>
+        <v>25</v>
       </c>
       <c r="D48" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49">
@@ -1218,14 +1218,14 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2025-06-29T18:00:00+00:00/PT1H</t>
+          <t>2025-06-29T20:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>23.88888888888889</v>
+        <v>26.66666666666667</v>
       </c>
       <c r="D49" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50">
@@ -1234,14 +1234,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2025-06-29T19:00:00+00:00/PT1H</t>
+          <t>2025-06-29T21:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>25.55555555555556</v>
+        <v>27.22222222222222</v>
       </c>
       <c r="D50" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51">
@@ -1250,14 +1250,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2025-06-29T20:00:00+00:00/PT1H</t>
+          <t>2025-06-29T23:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>27.22222222222222</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D51" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52">
@@ -1266,14 +1266,14 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2025-06-29T21:00:00+00:00/PT2H</t>
+          <t>2025-06-30T00:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>27.77777777777778</v>
+        <v>25</v>
       </c>
       <c r="D52" t="n">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53">
@@ -1282,14 +1282,14 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2025-06-29T23:00:00+00:00/PT1H</t>
+          <t>2025-06-30T01:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>26.66666666666667</v>
+        <v>23.88888888888889</v>
       </c>
       <c r="D53" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54">
@@ -1298,14 +1298,14 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2025-06-30T00:00:00+00:00/PT1H</t>
+          <t>2025-06-30T02:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>25.55555555555556</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="D54" t="n">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55">
@@ -1314,14 +1314,14 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2025-06-30T01:00:00+00:00/PT1H</t>
+          <t>2025-06-30T03:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>23.88888888888889</v>
+        <v>21.11111111111111</v>
       </c>
       <c r="D55" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56">
@@ -1330,14 +1330,14 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2025-06-30T02:00:00+00:00/PT1H</t>
+          <t>2025-06-30T04:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>22.22222222222222</v>
+        <v>20.55555555555556</v>
       </c>
       <c r="D56" t="n">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57">
@@ -1346,14 +1346,14 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2025-06-30T03:00:00+00:00/PT1H</t>
+          <t>2025-06-30T05:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>21.11111111111111</v>
+        <v>20</v>
       </c>
       <c r="D57" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58">
@@ -1362,14 +1362,14 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2025-06-30T04:00:00+00:00/PT1H</t>
+          <t>2025-06-30T06:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>20</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D58" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59">
@@ -1378,14 +1378,14 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2025-06-30T05:00:00+00:00/PT1H</t>
+          <t>2025-06-30T07:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>19.44444444444444</v>
+        <v>18.88888888888889</v>
       </c>
       <c r="D59" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60">
@@ -1394,14 +1394,14 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2025-06-30T06:00:00+00:00/PT2H</t>
+          <t>2025-06-30T09:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>18.88888888888889</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D60" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61">
@@ -1410,14 +1410,14 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2025-06-30T08:00:00+00:00/PT1H</t>
+          <t>2025-06-30T10:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>18.33333333333333</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D61" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62">
@@ -1426,14 +1426,14 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-06-30T09:00:00+00:00/PT2H</t>
+          <t>2025-06-30T11:00:00+00:00/PT3H</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>17.77777777777778</v>
+        <v>17.22222222222222</v>
       </c>
       <c r="D62" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63">
@@ -1442,14 +1442,14 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2025-06-30T11:00:00+00:00/PT3H</t>
+          <t>2025-06-30T14:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>17.22222222222222</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D63" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64">
@@ -1458,14 +1458,14 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2025-06-30T14:00:00+00:00/PT1H</t>
+          <t>2025-06-30T15:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>17.77777777777778</v>
+        <v>18.88888888888889</v>
       </c>
       <c r="D64" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="65">
@@ -1474,14 +1474,14 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2025-06-30T15:00:00+00:00/PT1H</t>
+          <t>2025-06-30T16:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>18.33333333333333</v>
+        <v>20</v>
       </c>
       <c r="D65" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66">
@@ -1490,14 +1490,14 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2025-06-30T16:00:00+00:00/PT1H</t>
+          <t>2025-06-30T17:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>20</v>
+        <v>21.66666666666667</v>
       </c>
       <c r="D66" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67">
@@ -1506,14 +1506,14 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2025-06-30T17:00:00+00:00/PT1H</t>
+          <t>2025-06-30T18:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>21.66666666666667</v>
+        <v>22.77777777777778</v>
       </c>
       <c r="D67" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="68">
@@ -1522,14 +1522,14 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2025-06-30T18:00:00+00:00/PT1H</t>
+          <t>2025-06-30T19:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>23.33333333333333</v>
+        <v>24.44444444444444</v>
       </c>
       <c r="D68" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69">
@@ -1538,14 +1538,14 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2025-06-30T19:00:00+00:00/PT1H</t>
+          <t>2025-06-30T20:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>25</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D69" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70">
@@ -1554,14 +1554,14 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2025-06-30T20:00:00+00:00/PT1H</t>
+          <t>2025-06-30T21:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>26.66666666666667</v>
+        <v>27.22222222222222</v>
       </c>
       <c r="D70" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71">
@@ -1570,14 +1570,14 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2025-06-30T21:00:00+00:00/PT2H</t>
+          <t>2025-06-30T23:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>27.22222222222222</v>
+        <v>26.66666666666667</v>
       </c>
       <c r="D71" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72">
@@ -1586,14 +1586,14 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2025-06-30T23:00:00+00:00/PT1H</t>
+          <t>2025-07-01T00:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>26.11111111111111</v>
+        <v>25</v>
       </c>
       <c r="D72" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73">
@@ -1602,14 +1602,14 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2025-07-01T00:00:00+00:00/PT1H</t>
+          <t>2025-07-01T01:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>25</v>
+        <v>23.33333333333333</v>
       </c>
       <c r="D73" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="74">
@@ -1618,14 +1618,14 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2025-07-01T01:00:00+00:00/PT1H</t>
+          <t>2025-07-01T02:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>23.33333333333333</v>
+        <v>21.66666666666667</v>
       </c>
       <c r="D74" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75">
@@ -1634,14 +1634,14 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2025-07-01T02:00:00+00:00/PT1H</t>
+          <t>2025-07-01T03:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>21.66666666666667</v>
+        <v>20</v>
       </c>
       <c r="D75" t="n">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76">
@@ -1650,14 +1650,14 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2025-07-01T03:00:00+00:00/PT1H</t>
+          <t>2025-07-01T04:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>20.55555555555556</v>
+        <v>18.88888888888889</v>
       </c>
       <c r="D76" t="n">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77">
@@ -1666,14 +1666,14 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2025-07-01T04:00:00+00:00/PT1H</t>
+          <t>2025-07-01T05:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>19.44444444444444</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D77" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78">
@@ -1682,14 +1682,14 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2025-07-01T05:00:00+00:00/PT1H</t>
+          <t>2025-07-01T07:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>18.88888888888889</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D78" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79">
@@ -1698,14 +1698,14 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2025-07-01T06:00:00+00:00/PT2H</t>
+          <t>2025-07-01T08:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>18.33333333333333</v>
+        <v>17.22222222222222</v>
       </c>
       <c r="D79" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="80">
@@ -1714,14 +1714,14 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2025-07-01T08:00:00+00:00/PT1H</t>
+          <t>2025-07-01T09:00:00+00:00/PT4H</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>17.77777777777778</v>
+        <v>16.66666666666667</v>
       </c>
       <c r="D80" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2025-07-01T09:00:00+00:00/PT1H</t>
+          <t>2025-07-01T13:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1746,14 +1746,14 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2025-07-01T10:00:00+00:00/PT3H</t>
+          <t>2025-07-01T15:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>16.66666666666667</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D82" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83">
@@ -1762,14 +1762,14 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2025-07-01T13:00:00+00:00/PT1H</t>
+          <t>2025-07-01T16:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>17.22222222222222</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D83" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="84">
@@ -1778,14 +1778,14 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2025-07-01T14:00:00+00:00/PT1H</t>
+          <t>2025-07-01T17:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>17.77777777777778</v>
+        <v>20.55555555555556</v>
       </c>
       <c r="D84" t="n">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85">
@@ -1794,14 +1794,14 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2025-07-01T15:00:00+00:00/PT1H</t>
+          <t>2025-07-01T18:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>18.33333333333333</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="D85" t="n">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="86">
@@ -1810,14 +1810,14 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2025-07-01T16:00:00+00:00/PT1H</t>
+          <t>2025-07-01T19:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>19.44444444444444</v>
+        <v>23.88888888888889</v>
       </c>
       <c r="D86" t="n">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87">
@@ -1826,14 +1826,14 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2025-07-01T17:00:00+00:00/PT1H</t>
+          <t>2025-07-01T20:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>21.11111111111111</v>
+        <v>25.55555555555556</v>
       </c>
       <c r="D87" t="n">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88">
@@ -1842,14 +1842,14 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2025-07-01T18:00:00+00:00/PT1H</t>
+          <t>2025-07-01T21:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>22.77777777777778</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D88" t="n">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="89">
@@ -1858,14 +1858,14 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2025-07-01T19:00:00+00:00/PT1H</t>
+          <t>2025-07-01T23:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>24.44444444444444</v>
+        <v>25.55555555555556</v>
       </c>
       <c r="D89" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="90">
@@ -1874,14 +1874,14 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2025-07-01T20:00:00+00:00/PT1H</t>
+          <t>2025-07-02T00:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>26.11111111111111</v>
+        <v>24.44444444444444</v>
       </c>
       <c r="D90" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91">
@@ -1890,14 +1890,14 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2025-07-01T21:00:00+00:00/PT2H</t>
+          <t>2025-07-02T01:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>27.22222222222222</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="D91" t="n">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92">
@@ -1906,14 +1906,14 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2025-07-01T23:00:00+00:00/PT1H</t>
+          <t>2025-07-02T02:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>26.66666666666667</v>
+        <v>20.55555555555556</v>
       </c>
       <c r="D92" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="93">
@@ -1922,14 +1922,14 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2025-07-02T00:00:00+00:00/PT1H</t>
+          <t>2025-07-02T03:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>25</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D93" t="n">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="94">
@@ -1938,14 +1938,14 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2025-07-02T01:00:00+00:00/PT1H</t>
+          <t>2025-07-02T04:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>23.33333333333333</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D94" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="95">
@@ -1954,14 +1954,14 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2025-07-02T02:00:00+00:00/PT1H</t>
+          <t>2025-07-02T05:00:00+00:00/PT4H</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>21.66666666666667</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D95" t="n">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="96">
@@ -1970,14 +1970,14 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2025-07-02T03:00:00+00:00/PT1H</t>
+          <t>2025-07-02T09:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>20.55555555555556</v>
+        <v>17.22222222222222</v>
       </c>
       <c r="D96" t="n">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97">
@@ -1986,14 +1986,14 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2025-07-02T04:00:00+00:00/PT2H</t>
+          <t>2025-07-02T11:00:00+00:00/PT3H</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>19.44444444444444</v>
+        <v>16.66666666666667</v>
       </c>
       <c r="D97" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="98">
@@ -2002,14 +2002,14 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2025-07-02T06:00:00+00:00/PT3H</t>
+          <t>2025-07-02T14:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>18.88888888888889</v>
+        <v>17.22222222222222</v>
       </c>
       <c r="D98" t="n">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="99">
@@ -2018,14 +2018,14 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2025-07-02T09:00:00+00:00/PT1H</t>
+          <t>2025-07-02T15:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>18.33333333333333</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D99" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100">
@@ -2034,14 +2034,14 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2025-07-02T10:00:00+00:00/PT2H</t>
+          <t>2025-07-02T16:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>17.77777777777778</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D100" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="101">
@@ -2050,14 +2050,14 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2025-07-02T12:00:00+00:00/PT2H</t>
+          <t>2025-07-02T17:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>17.22222222222222</v>
+        <v>21.11111111111111</v>
       </c>
       <c r="D101" t="n">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102">
@@ -2066,14 +2066,14 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2025-07-02T14:00:00+00:00/PT1H</t>
+          <t>2025-07-02T18:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>17.77777777777778</v>
+        <v>22.77777777777778</v>
       </c>
       <c r="D102" t="n">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="103">
@@ -2082,14 +2082,14 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2025-07-02T15:00:00+00:00/PT1H</t>
+          <t>2025-07-02T19:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>18.33333333333333</v>
+        <v>24.44444444444444</v>
       </c>
       <c r="D103" t="n">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="104">
@@ -2098,14 +2098,14 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2025-07-02T16:00:00+00:00/PT1H</t>
+          <t>2025-07-02T20:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>20</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D104" t="n">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="105">
@@ -2114,14 +2114,14 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2025-07-02T17:00:00+00:00/PT1H</t>
+          <t>2025-07-02T21:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>22.22222222222222</v>
+        <v>26.66666666666667</v>
       </c>
       <c r="D105" t="n">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106">
@@ -2130,14 +2130,14 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2025-07-02T18:00:00+00:00/PT1H</t>
+          <t>2025-07-02T23:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>23.88888888888889</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D106" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="107">
@@ -2146,14 +2146,14 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2025-07-02T19:00:00+00:00/PT1H</t>
+          <t>2025-07-03T00:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>25.55555555555556</v>
+        <v>24.44444444444444</v>
       </c>
       <c r="D107" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="108">
@@ -2162,14 +2162,14 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2025-07-02T20:00:00+00:00/PT1H</t>
+          <t>2025-07-03T01:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>26.66666666666667</v>
+        <v>22.77777777777778</v>
       </c>
       <c r="D108" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="109">
@@ -2178,14 +2178,14 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2025-07-02T21:00:00+00:00/PT2H</t>
+          <t>2025-07-03T02:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>27.22222222222222</v>
+        <v>21.66666666666667</v>
       </c>
       <c r="D109" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110">
@@ -2194,14 +2194,14 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2025-07-02T23:00:00+00:00/PT1H</t>
+          <t>2025-07-03T03:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>26.66666666666667</v>
+        <v>20</v>
       </c>
       <c r="D110" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="111">
@@ -2210,14 +2210,14 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2025-07-03T00:00:00+00:00/PT1H</t>
+          <t>2025-07-03T04:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>25.55555555555556</v>
+        <v>18.88888888888889</v>
       </c>
       <c r="D111" t="n">
-        <v>78</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112">
@@ -2226,14 +2226,14 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2025-07-03T01:00:00+00:00/PT1H</t>
+          <t>2025-07-03T05:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>23.88888888888889</v>
+        <v>18.33333333333333</v>
       </c>
       <c r="D112" t="n">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113">
@@ -2242,14 +2242,14 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2025-07-03T02:00:00+00:00/PT1H</t>
+          <t>2025-07-03T06:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>22.22222222222222</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D113" t="n">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="114">
@@ -2258,14 +2258,14 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2025-07-03T03:00:00+00:00/PT1H</t>
+          <t>2025-07-03T08:00:00+00:00/PT7H</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>20.55555555555556</v>
+        <v>17.22222222222222</v>
       </c>
       <c r="D114" t="n">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="115">
@@ -2274,14 +2274,14 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2025-07-03T04:00:00+00:00/PT2H</t>
+          <t>2025-07-03T15:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>19.44444444444444</v>
+        <v>17.77777777777778</v>
       </c>
       <c r="D115" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="116">
@@ -2290,14 +2290,14 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2025-07-03T06:00:00+00:00/PT3H</t>
+          <t>2025-07-03T16:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>18.88888888888889</v>
+        <v>19.44444444444444</v>
       </c>
       <c r="D116" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117">
@@ -2306,14 +2306,14 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2025-07-03T09:00:00+00:00/PT2H</t>
+          <t>2025-07-03T17:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>18.33333333333333</v>
+        <v>21.11111111111111</v>
       </c>
       <c r="D117" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="118">
@@ -2322,14 +2322,14 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2025-07-03T11:00:00+00:00/PT3H</t>
+          <t>2025-07-03T18:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>17.77777777777778</v>
+        <v>22.77777777777778</v>
       </c>
       <c r="D118" t="n">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="119">
@@ -2338,14 +2338,14 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2025-07-03T14:00:00+00:00/PT1H</t>
+          <t>2025-07-03T19:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>18.33333333333333</v>
+        <v>24.44444444444444</v>
       </c>
       <c r="D119" t="n">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="120">
@@ -2354,14 +2354,14 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2025-07-03T15:00:00+00:00/PT1H</t>
+          <t>2025-07-03T20:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>18.88888888888889</v>
+        <v>25.55555555555556</v>
       </c>
       <c r="D120" t="n">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="121">
@@ -2370,14 +2370,14 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2025-07-03T16:00:00+00:00/PT1H</t>
+          <t>2025-07-03T21:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>20.55555555555556</v>
+        <v>26.11111111111111</v>
       </c>
       <c r="D121" t="n">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="122">
@@ -2386,14 +2386,14 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>2025-07-03T17:00:00+00:00/PT1H</t>
+          <t>2025-07-03T23:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>21.66666666666667</v>
+        <v>25.55555555555556</v>
       </c>
       <c r="D122" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="123">
@@ -2402,14 +2402,14 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>2025-07-03T18:00:00+00:00/PT1H</t>
+          <t>2025-07-04T00:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>23.33333333333333</v>
+        <v>24.44444444444444</v>
       </c>
       <c r="D123" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124">
@@ -2418,14 +2418,14 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>2025-07-03T19:00:00+00:00/PT1H</t>
+          <t>2025-07-04T01:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>25</v>
+        <v>22.77777777777778</v>
       </c>
       <c r="D124" t="n">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="125">
@@ -2434,14 +2434,14 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2025-07-03T20:00:00+00:00/PT1H</t>
+          <t>2025-07-04T02:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>26.11111111111111</v>
+        <v>21.11111111111111</v>
       </c>
       <c r="D125" t="n">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="126">
@@ -2450,14 +2450,14 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2025-07-03T21:00:00+00:00/PT2H</t>
+          <t>2025-07-04T03:00:00+00:00/PT1H</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>26.66666666666667</v>
+        <v>20</v>
       </c>
       <c r="D126" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="127">
@@ -2466,14 +2466,14 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2025-07-03T23:00:00+00:00/PT1H</t>
+          <t>2025-07-04T04:00:00+00:00/PT2H</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>26.11111111111111</v>
+        <v>18.88888888888889</v>
       </c>
       <c r="D127" t="n">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="128">
@@ -2482,14 +2482,190 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2025-07-04T00:00:00+00:00/PT1H</t>
+          <t>2025-07-04T06:00:00+00:00/PT3H</t>
         </is>
       </c>
       <c r="C128" t="n">
+        <v>18.33333333333333</v>
+      </c>
+      <c r="D128" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>2025-07-04T09:00:00+00:00/PT4H</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>17.77777777777778</v>
+      </c>
+      <c r="D129" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>2025-07-04T13:00:00+00:00/PT2H</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>18.33333333333333</v>
+      </c>
+      <c r="D130" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>2025-07-04T15:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>18.88888888888889</v>
+      </c>
+      <c r="D131" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>2025-07-04T16:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>20</v>
+      </c>
+      <c r="D132" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>2025-07-04T17:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>21.66666666666667</v>
+      </c>
+      <c r="D133" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>2025-07-04T18:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>22.77777777777778</v>
+      </c>
+      <c r="D134" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>2025-07-04T19:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
         <v>24.44444444444444</v>
       </c>
-      <c r="D128" t="n">
+      <c r="D135" t="n">
         <v>76</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>2025-07-04T20:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>26.11111111111111</v>
+      </c>
+      <c r="D136" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>2025-07-04T21:00:00+00:00/PT2H</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>26.66666666666667</v>
+      </c>
+      <c r="D137" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>2025-07-04T23:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>26.11111111111111</v>
+      </c>
+      <c r="D138" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>2025-07-05T00:00:00+00:00/PT1H</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>23.88888888888889</v>
+      </c>
+      <c r="D139" t="n">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>